<commit_message>
commit to switch and update database
</commit_message>
<xml_diff>
--- a/model/model/best_threshold.xlsx
+++ b/model/model/best_threshold.xlsx
@@ -49,7 +49,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -63,6 +63,13 @@
     </fill>
   </fills>
   <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -85,32 +92,25 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -482,37 +482,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>0.7842</v>
+        <v>0.973</v>
       </c>
       <c r="C2" s="4">
-        <v>0.9884000000000001</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.7399</v>
+        <v>0.9686</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>0.8734999999999999</v>
+        <v>0.5584</v>
       </c>
       <c r="F2" s="4">
-        <v>0.9107</v>
+        <v>0.7044</v>
       </c>
       <c r="G2" s="4">
-        <v>0.616</v>
+        <v>0.7933</v>
       </c>
       <c r="H2" s="4">
-        <v>0.9761</v>
+        <v>0.7587999999999999</v>
       </c>
       <c r="I2" s="4">
-        <v>0.9751000000000001</v>
+        <v>0.4669</v>
       </c>
       <c r="J2" s="4">
-        <v>0.7483</v>
+        <v>0.5740999999999999</v>
       </c>
       <c r="K2" s="4">
-        <v>0.7009000000000001</v>
+        <v>0.8813</v>
       </c>
       <c r="L2" s="4">
-        <v>0.83131</v>
+        <v>0.6678799999999999</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
@@ -520,37 +520,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>0.9314</v>
+        <v>0.7426</v>
       </c>
       <c r="C3" s="4">
-        <v>0.5644</v>
+        <v>0.6765</v>
       </c>
       <c r="D3" s="4">
-        <v>0.9151</v>
+        <v>0.9434</v>
       </c>
       <c r="E3" s="4">
-        <v>0.9216</v>
+        <v>0.9327</v>
       </c>
       <c r="F3" s="4">
-        <v>0.8148</v>
+        <v>0.8585</v>
       </c>
       <c r="G3" s="4">
-        <v>0.9505</v>
+        <v>0.9029</v>
       </c>
       <c r="H3" s="4">
-        <v>0.5965</v>
+        <v>0.8407</v>
       </c>
       <c r="I3" s="4">
-        <v>0.84</v>
+        <v>0.99</v>
       </c>
       <c r="J3" s="4">
-        <v>0.8824</v>
+        <v>0.98</v>
       </c>
       <c r="K3" s="4">
-        <v>0.902</v>
+        <v>0.89</v>
       </c>
       <c r="L3" s="4">
-        <v>0.83187</v>
+        <v>0.8757300000000001</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21">

</xml_diff>